<commit_message>
fixed clean up test data
</commit_message>
<xml_diff>
--- a/packages/meditrak-server/src/tests/testData/surveys/importANewSurvey.xlsx
+++ b/packages/meditrak-server/src/tests/testData/surveys/importANewSurvey.xlsx
@@ -5,22 +5,22 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Projects\tupaia\packages\meditrak-server\src\tests\testData\importSurveys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Projects\tupaia\packages\meditrak-server\src\tests\testData\surveys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7F1265-4FBC-4F58-A6C4-375D3D97DED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE38CF0D-FA2F-4CC6-BA0E-C23FC13A7D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test New Survey Import" sheetId="2" r:id="rId1"/>
+    <sheet name="test_new_survey_import 1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>code</t>
   </si>
@@ -67,25 +67,19 @@
     <t>detailLabel</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Sodium chloride 0.9% isotonic injectable solution</t>
-  </si>
-  <si>
-    <t>Sodium lactate,compound solution</t>
-  </si>
-  <si>
-    <t>Calcium gluconate 100mg/mL in 10mL ampoule injection</t>
-  </si>
-  <si>
-    <t>TEST_53ea14bfc_test</t>
-  </si>
-  <si>
-    <t>TEST_53d544bfc_test</t>
-  </si>
-  <si>
-    <t>TEST_398ac4bfc_test</t>
+    <t>FreeText</t>
+  </si>
+  <si>
+    <t>fdfuu42a22321c123a8_test</t>
+  </si>
+  <si>
+    <t>Test question fdfuu42a22321c123a8_test</t>
+  </si>
+  <si>
+    <t>fdfzz42a66321c123a8_test</t>
+  </si>
+  <si>
+    <t>Test question fdfzz42a66321c123a8_test</t>
   </si>
 </sst>
 </file>
@@ -487,7 +481,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -541,16 +535,16 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -566,16 +560,16 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -590,18 +584,10 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>

</xml_diff>

<commit_message>
cleaned up test data
</commit_message>
<xml_diff>
--- a/packages/meditrak-server/src/tests/testData/surveys/importANewSurvey.xlsx
+++ b/packages/meditrak-server/src/tests/testData/surveys/importANewSurvey.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Projects\tupaia\packages\meditrak-server\src\tests\testData\surveys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE38CF0D-FA2F-4CC6-BA0E-C23FC13A7D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C384F0-470A-4A55-B165-844296EE0D04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test_new_survey_import 1" sheetId="2" r:id="rId1"/>
+    <sheet name="new_survey_import_1_test" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -481,7 +481,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>